<commit_message>
Wrote some sSSY results
</commit_message>
<xml_diff>
--- a/Data/Other SSY studies.xlsx
+++ b/Data/Other SSY studies.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="120">
   <si>
     <t>Author</t>
   </si>
@@ -468,11 +469,107 @@
   <si>
     <t>105 x 10**6</t>
   </si>
+  <si>
+    <t>High Mountian</t>
+  </si>
+  <si>
+    <t>Q = (280)A**0.46</t>
+  </si>
+  <si>
+    <t>Q = (12)A**0.42</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>max watershed elev</t>
+  </si>
+  <si>
+    <t>500-1,000 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,000-3,000 m </t>
+  </si>
+  <si>
+    <t>&gt;3,000 m</t>
+  </si>
+  <si>
+    <t>100-500 m</t>
+  </si>
+  <si>
+    <t>&lt;100 m</t>
+  </si>
+  <si>
+    <t>Q = (8)A**0.66</t>
+  </si>
+  <si>
+    <t>Q = (1)A**0.64</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>sediment load (Qs)=cA**d (Milliman 1992)</t>
+  </si>
+  <si>
+    <t>TOTAL A</t>
+  </si>
+  <si>
+    <t>TOTAL Qs</t>
+  </si>
+  <si>
+    <t>UPPER A km2</t>
+  </si>
+  <si>
+    <t>UPPER Qs tons/year</t>
+  </si>
+  <si>
+    <t>Q = (65)A**0.56 (Area 2: S. Asia, Oceania)</t>
+  </si>
+  <si>
+    <t>SSY</t>
+  </si>
+  <si>
+    <t>sSSY</t>
+  </si>
+  <si>
+    <t>Milliman 1992 Table 2</t>
+  </si>
+  <si>
+    <t>sediment load (Y)=cA**f (Milliman 1992)</t>
+  </si>
+  <si>
+    <t>Q = (280)A**-0.54</t>
+  </si>
+  <si>
+    <t>Q = (65)A**-0.46 (Area 2: S. Asia, Oceania)</t>
+  </si>
+  <si>
+    <t>Q = (12)A**-0.59</t>
+  </si>
+  <si>
+    <t>Q = (8)A**-0.34</t>
+  </si>
+  <si>
+    <t>Q = (5)A**-0.20</t>
+  </si>
+  <si>
+    <t>UPPER sSSY tons/km2/year</t>
+  </si>
+  <si>
+    <t>TOTAL sSSY tons/km2/year</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -525,12 +622,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,6 +644,163 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>437138</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180469</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3067050"/>
+          <a:ext cx="5275838" cy="2637919"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>551376</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>227969</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10905051" y="180975"/>
+          <a:ext cx="3334193" cy="2705100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590029</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>123215</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5362575" y="3057525"/>
+          <a:ext cx="4171429" cy="4876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>399543</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>123214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9744075" y="3048000"/>
+          <a:ext cx="4057143" cy="4885714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -814,10 +1069,10 @@
   <dimension ref="B2:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,4 +1650,393 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5">
+        <v>280</v>
+      </c>
+      <c r="E5">
+        <v>0.46</v>
+      </c>
+      <c r="F5">
+        <f>0.9</f>
+        <v>0.9</v>
+      </c>
+      <c r="G5" s="5">
+        <f>D5*(F5^E5)</f>
+        <v>266.75316788440239</v>
+      </c>
+      <c r="H5">
+        <v>1.78</v>
+      </c>
+      <c r="I5" s="4">
+        <f>D5*(H5^E5)</f>
+        <v>365.04905826237916</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6">
+        <v>65</v>
+      </c>
+      <c r="E6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F9" si="0">0.9</f>
+        <v>0.9</v>
+      </c>
+      <c r="G6" s="5">
+        <f>D6*(F6^E6)</f>
+        <v>61.275824259262698</v>
+      </c>
+      <c r="H6">
+        <v>1.78</v>
+      </c>
+      <c r="I6" s="4">
+        <f>D6*(H6^E6)</f>
+        <v>89.773582804517957</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>0.42</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="G7" s="5">
+        <f>D7*(F7^E7)</f>
+        <v>11.48056072353037</v>
+      </c>
+      <c r="H7">
+        <v>1.78</v>
+      </c>
+      <c r="I7" s="4">
+        <f>D7*(H7^E7)</f>
+        <v>15.288245463923166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>0.66</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="G8" s="5">
+        <f>D8*(F8^E8)</f>
+        <v>7.4625979282461516</v>
+      </c>
+      <c r="H8">
+        <v>1.78</v>
+      </c>
+      <c r="I8" s="4">
+        <f>D8*(H8^E8)</f>
+        <v>11.704886007638859</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0.64</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="G9" s="5">
+        <f>D9*(F9^E9)</f>
+        <v>0.93479247142821487</v>
+      </c>
+      <c r="H9">
+        <v>1.78</v>
+      </c>
+      <c r="I9" s="4">
+        <f>D9*(H9^E9)</f>
+        <v>1.4463346856649641</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12">
+        <v>280</v>
+      </c>
+      <c r="E12">
+        <v>-0.54</v>
+      </c>
+      <c r="F12">
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="4">
+        <f>D12*(F12^E12)</f>
+        <v>296.3924087604471</v>
+      </c>
+      <c r="H12">
+        <v>1.78</v>
+      </c>
+      <c r="I12" s="4">
+        <f>D12*(H12^E12)</f>
+        <v>205.0837405968422</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13">
+        <v>65</v>
+      </c>
+      <c r="E13">
+        <v>-0.46</v>
+      </c>
+      <c r="F13">
+        <v>0.9</v>
+      </c>
+      <c r="G13" s="4">
+        <f>D13*(F13^E13)</f>
+        <v>68.227868273665564</v>
+      </c>
+      <c r="H13">
+        <v>1.78</v>
+      </c>
+      <c r="I13" s="4">
+        <f>D13*(H13^E13)</f>
+        <v>49.856312701178759</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>-0.59</v>
+      </c>
+      <c r="F14">
+        <v>0.9</v>
+      </c>
+      <c r="G14" s="4">
+        <f>D14*(F14^E14)</f>
+        <v>12.769625639933327</v>
+      </c>
+      <c r="H14">
+        <v>1.78</v>
+      </c>
+      <c r="I14" s="4">
+        <f>D14*(H14^E14)</f>
+        <v>8.5395196986982409</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>-0.34</v>
+      </c>
+      <c r="F15">
+        <v>0.9</v>
+      </c>
+      <c r="G15" s="4">
+        <f>D15*(F15^E15)</f>
+        <v>8.2917754758290574</v>
+      </c>
+      <c r="H15">
+        <v>1.78</v>
+      </c>
+      <c r="I15" s="4">
+        <f>D15*(H15^E15)</f>
+        <v>6.5757786559768858</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>-0.2</v>
+      </c>
+      <c r="F16">
+        <v>0.9</v>
+      </c>
+      <c r="G16" s="4">
+        <f>D16*(F16^E16)</f>
+        <v>5.1064784380006758</v>
+      </c>
+      <c r="H16">
+        <v>1.78</v>
+      </c>
+      <c r="I16" s="4">
+        <f>D16*(H16^E16)</f>
+        <v>4.455392853208485</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
writing up annual SSY estimates
</commit_message>
<xml_diff>
--- a/Data/Other SSY studies.xlsx
+++ b/Data/Other SSY studies.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="129">
   <si>
     <t>Author</t>
   </si>
@@ -562,13 +562,40 @@
   <si>
     <t>TOTAL sSSY tons/km2/year</t>
   </si>
+  <si>
+    <t>Hettler 1997</t>
+  </si>
+  <si>
+    <t>Ok Tedi, PNG</t>
+  </si>
+  <si>
+    <t>Ningerum</t>
+  </si>
+  <si>
+    <t>Konkonda</t>
+  </si>
+  <si>
+    <t>citing Eagle and Higgins 1991</t>
+  </si>
+  <si>
+    <t>Upland</t>
+  </si>
+  <si>
+    <t>Mountain (Oceania)</t>
+  </si>
+  <si>
+    <t>Lowland</t>
+  </si>
+  <si>
+    <t>Coastal Plain</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -593,12 +620,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -622,13 +655,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1066,19 +1101,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J28"/>
+  <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
@@ -1448,201 +1483,234 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="4">
-        <v>76000</v>
-      </c>
-      <c r="G18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" t="s">
-        <v>84</v>
-      </c>
-      <c r="J18" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="4">
-        <v>35000</v>
-      </c>
-      <c r="G19" t="s">
-        <v>88</v>
+        <v>121</v>
+      </c>
+      <c r="G19" s="4">
+        <v>40000</v>
+      </c>
+      <c r="I19" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D20" s="4"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22">
-        <v>42.9</v>
-      </c>
-      <c r="F22">
-        <v>61.2</v>
-      </c>
-      <c r="G22">
-        <v>2630</v>
-      </c>
-      <c r="H22">
-        <v>0.08</v>
-      </c>
-      <c r="J22" t="s">
-        <v>21</v>
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" s="4">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="4">
+        <v>6900000</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" t="s">
-        <v>31</v>
+        <v>85</v>
+      </c>
+      <c r="D23" s="4">
+        <v>76000</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" t="s">
-        <v>40</v>
+        <v>87</v>
+      </c>
+      <c r="I23" t="s">
+        <v>84</v>
       </c>
       <c r="J23" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" t="s">
-        <v>32</v>
+        <v>86</v>
+      </c>
+      <c r="D24" s="4">
+        <v>35000</v>
       </c>
       <c r="G24" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" t="s">
-        <v>41</v>
-      </c>
-      <c r="J24" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" t="s">
-        <v>42</v>
-      </c>
-      <c r="J25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" t="s">
-        <v>43</v>
-      </c>
-      <c r="J26" t="s">
-        <v>47</v>
-      </c>
+      <c r="D25" s="4"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
       </c>
       <c r="D27">
-        <v>82</v>
-      </c>
-      <c r="F27" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" t="s">
-        <v>38</v>
+        <v>42.9</v>
+      </c>
+      <c r="F27">
+        <v>61.2</v>
+      </c>
+      <c r="G27">
+        <v>2630</v>
       </c>
       <c r="H27">
-        <v>0.13</v>
+        <v>0.08</v>
       </c>
       <c r="J27" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" t="s">
+        <v>42</v>
+      </c>
+      <c r="J30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" t="s">
+        <v>43</v>
+      </c>
+      <c r="J31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>82</v>
+      </c>
+      <c r="F32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32">
+        <v>0.13</v>
+      </c>
+      <c r="J32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33">
         <v>38.799999999999997</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F33" t="s">
         <v>36</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G33" t="s">
         <v>39</v>
       </c>
-      <c r="H28">
+      <c r="H33">
         <v>0.76</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J33" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1656,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,6 +1991,9 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
       <c r="B13" t="s">
         <v>95</v>
       </c>
@@ -1951,34 +2022,40 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="A14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>12</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <v>-0.59</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <v>0.9</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="7">
         <f>D14*(F14^E14)</f>
         <v>12.769625639933327</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="6">
         <v>1.78</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="7">
         <f>D14*(H14^E14)</f>
         <v>8.5395196986982409</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>127</v>
+      </c>
       <c r="B15" t="s">
         <v>97</v>
       </c>
@@ -2007,6 +2084,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>128</v>
+      </c>
       <c r="B16" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
revised up to end of results
</commit_message>
<xml_diff>
--- a/Data/Other SSY studies.xlsx
+++ b/Data/Other SSY studies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SSY watersheds" sheetId="1" r:id="rId1"/>
@@ -2235,7 +2235,7 @@
   <dimension ref="B2:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:C25"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Almost done with Trents last revisions
still need to work on Discussion and read over it
</commit_message>
<xml_diff>
--- a/Data/Other SSY studies.xlsx
+++ b/Data/Other SSY studies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SSY watersheds" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="164">
   <si>
     <t>Author</t>
   </si>
@@ -540,9 +540,6 @@
     <t>Milliman 1992 Table 2</t>
   </si>
   <si>
-    <t>sediment load (Y)=cA**f (Milliman 1992)</t>
-  </si>
-  <si>
     <t>Q = (280)A**-0.54</t>
   </si>
   <si>
@@ -688,6 +685,15 @@
   </si>
   <si>
     <t>Mg/km2</t>
+  </si>
+  <si>
+    <t>sediment yield (Y)=cA**f (Milliman 1992)</t>
+  </si>
+  <si>
+    <t>UPPER A km2 x 10^6</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -796,14 +802,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>143289</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>437138</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>180469</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114208</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -820,8 +826,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3067050"/>
-          <a:ext cx="5275838" cy="2637919"/>
+          <a:off x="0" y="3572289"/>
+          <a:ext cx="5274181" cy="2637919"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -832,14 +838,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>551376</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>227969</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>227968</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
@@ -871,15 +877,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>573571</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>108916</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>590029</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>123215</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1070421</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>32106</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -896,8 +902,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5362575" y="3057525"/>
-          <a:ext cx="4171429" cy="4876190"/>
+          <a:off x="5410614" y="3537916"/>
+          <a:ext cx="4182611" cy="4876190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -908,16 +914,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1308652</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>399543</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>123214</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>117934</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>189475</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -934,8 +940,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9744075" y="3048000"/>
-          <a:ext cx="4057143" cy="4885714"/>
+          <a:off x="9831456" y="3495261"/>
+          <a:ext cx="4077021" cy="4885714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1594,10 +1600,10 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" t="s">
         <v>120</v>
-      </c>
-      <c r="C19" t="s">
-        <v>121</v>
       </c>
       <c r="G19" s="4">
         <v>40000</v>
@@ -1608,10 +1614,10 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G20" s="4">
         <v>300000</v>
@@ -1619,7 +1625,7 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G21" s="4">
         <v>6900000</v>
@@ -1831,10 +1837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I16"/>
+  <dimension ref="A2:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,21 +1849,22 @@
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="38.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -1877,16 +1884,19 @@
         <v>106</v>
       </c>
       <c r="G4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H4" t="s">
         <v>107</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>104</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -1906,19 +1916,23 @@
         <f>0.9</f>
         <v>0.9</v>
       </c>
-      <c r="G5" s="5">
-        <f>D5*(F5^E5)</f>
-        <v>266.75316788440239</v>
-      </c>
-      <c r="H5">
+      <c r="G5">
+        <f>F5/10^6</f>
+        <v>9.0000000000000007E-7</v>
+      </c>
+      <c r="H5" s="5">
+        <f>D5*(G5^E5)</f>
+        <v>0.46356387622103573</v>
+      </c>
+      <c r="I5">
         <v>1.78</v>
       </c>
-      <c r="I5" s="4">
-        <f>D5*(H5^E5)</f>
+      <c r="J5" s="4">
+        <f>D5*(I5^E5)</f>
         <v>365.04905826237916</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>95</v>
       </c>
@@ -1935,19 +1949,23 @@
         <f t="shared" ref="F6:F9" si="0">0.9</f>
         <v>0.9</v>
       </c>
-      <c r="G6" s="5">
-        <f>D6*(F6^E6)</f>
-        <v>61.275824259262698</v>
-      </c>
-      <c r="H6">
+      <c r="G6">
+        <f t="shared" ref="G6:G9" si="1">F6/10^6</f>
+        <v>9.0000000000000007E-7</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" ref="H6:H9" si="2">D6*(G6^E6)</f>
+        <v>2.6747867422734186E-2</v>
+      </c>
+      <c r="I6">
         <v>1.78</v>
       </c>
-      <c r="I6" s="4">
-        <f>D6*(H6^E6)</f>
+      <c r="J6" s="4">
+        <f>D6*(I6^E6)</f>
         <v>89.773582804517957</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>94</v>
       </c>
@@ -1964,19 +1982,23 @@
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="G7" s="5">
-        <f>D7*(F7^E7)</f>
-        <v>11.48056072353037</v>
-      </c>
-      <c r="H7">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>9.0000000000000007E-7</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="2"/>
+        <v>3.4670739108205353E-2</v>
+      </c>
+      <c r="I7">
         <v>1.78</v>
       </c>
-      <c r="I7" s="4">
-        <f>D7*(H7^E7)</f>
+      <c r="J7" s="4">
+        <f>D7*(I7^E7)</f>
         <v>15.288245463923166</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>97</v>
       </c>
@@ -1993,19 +2015,23 @@
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="G8" s="5">
-        <f>D8*(F8^E8)</f>
-        <v>7.4625979282461516</v>
-      </c>
-      <c r="H8">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>9.0000000000000007E-7</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="2"/>
+        <v>8.1825759149052049E-4</v>
+      </c>
+      <c r="I8">
         <v>1.78</v>
       </c>
-      <c r="I8" s="4">
-        <f>D8*(H8^E8)</f>
+      <c r="J8" s="4">
+        <f>D8*(I8^E8)</f>
         <v>11.704886007638859</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>98</v>
       </c>
@@ -2022,24 +2048,28 @@
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="G9" s="5">
-        <f>D9*(F9^E9)</f>
-        <v>0.93479247142821487</v>
-      </c>
-      <c r="H9">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>9.0000000000000007E-7</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="2"/>
+        <v>1.3511862155962171E-4</v>
+      </c>
+      <c r="I9">
         <v>1.78</v>
       </c>
-      <c r="I9" s="4">
-        <f>D9*(H9^E9)</f>
+      <c r="J9" s="4">
+        <f>D9*(I9^E9)</f>
         <v>1.4463346856649641</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -2047,28 +2077,31 @@
         <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
       <c r="D11" t="s">
         <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
       <c r="F11" t="s">
         <v>106</v>
       </c>
       <c r="G11" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I11" t="s">
+        <v>104</v>
+      </c>
+      <c r="J11" t="s">
         <v>118</v>
       </c>
-      <c r="H11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -2076,7 +2109,7 @@
         <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12">
         <v>280</v>
@@ -2087,27 +2120,31 @@
       <c r="F12">
         <v>0.9</v>
       </c>
-      <c r="G12" s="4">
-        <f>D12*(F12^E12)</f>
-        <v>296.3924087604471</v>
-      </c>
-      <c r="H12">
+      <c r="G12">
+        <f>F12/10^6</f>
+        <v>9.0000000000000007E-7</v>
+      </c>
+      <c r="H12" s="4">
+        <f>D12*(G12^E12)</f>
+        <v>515070.97357892909</v>
+      </c>
+      <c r="I12">
         <v>1.78</v>
       </c>
-      <c r="I12" s="4">
-        <f>D12*(H12^E12)</f>
+      <c r="J12" s="4">
+        <f>D12*(I12^E12)</f>
         <v>205.0837405968422</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
         <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13">
         <v>65</v>
@@ -2118,27 +2155,31 @@
       <c r="F13">
         <v>0.9</v>
       </c>
-      <c r="G13" s="4">
-        <f>D13*(F13^E13)</f>
-        <v>68.227868273665564</v>
-      </c>
-      <c r="H13">
+      <c r="G13">
+        <f t="shared" ref="G13:G16" si="3">F13/10^6</f>
+        <v>9.0000000000000007E-7</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" ref="H13:H16" si="4">D13*(G13^E13)</f>
+        <v>39261.040244045907</v>
+      </c>
+      <c r="I13">
         <v>1.78</v>
       </c>
-      <c r="I13" s="4">
-        <f>D13*(H13^E13)</f>
+      <c r="J13" s="4">
+        <f>D13*(I13^E13)</f>
         <v>49.856312701178759</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>94</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D14" s="6">
         <v>12</v>
@@ -2149,27 +2190,31 @@
       <c r="F14" s="6">
         <v>0.9</v>
       </c>
-      <c r="G14" s="7">
-        <f>D14*(F14^E14)</f>
-        <v>12.769625639933327</v>
-      </c>
-      <c r="H14" s="6">
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>9.0000000000000007E-7</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="4"/>
+        <v>44276.997758483747</v>
+      </c>
+      <c r="I14" s="6">
         <v>1.78</v>
       </c>
-      <c r="I14" s="7">
-        <f>D14*(H14^E14)</f>
+      <c r="J14" s="7">
+        <f>D14*(I14^E14)</f>
         <v>8.5395196986982409</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
         <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15">
         <v>8</v>
@@ -2180,27 +2225,31 @@
       <c r="F15">
         <v>0.9</v>
       </c>
-      <c r="G15" s="4">
-        <f>D15*(F15^E15)</f>
-        <v>8.2917754758290574</v>
-      </c>
-      <c r="H15">
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>9.0000000000000007E-7</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="4"/>
+        <v>909.17510165613464</v>
+      </c>
+      <c r="I15">
         <v>1.78</v>
       </c>
-      <c r="I15" s="4">
-        <f>D15*(H15^E15)</f>
+      <c r="J15" s="4">
+        <f>D15*(I15^E15)</f>
         <v>6.5757786559768858</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B16" t="s">
         <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -2211,15 +2260,19 @@
       <c r="F16">
         <v>0.9</v>
       </c>
-      <c r="G16" s="4">
-        <f>D16*(F16^E16)</f>
-        <v>5.1064784380006758</v>
-      </c>
-      <c r="H16">
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>9.0000000000000007E-7</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="4"/>
+        <v>80.932229138367319</v>
+      </c>
+      <c r="I16">
         <v>1.78</v>
       </c>
-      <c r="I16" s="4">
-        <f>D16*(H16^E16)</f>
+      <c r="J16" s="4">
+        <f>D16*(I16^E16)</f>
         <v>4.455392853208485</v>
       </c>
     </row>
@@ -2234,7 +2287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -2248,46 +2301,46 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" t="s">
         <v>135</v>
       </c>
-      <c r="C6" t="s">
-        <v>136</v>
-      </c>
       <c r="E6" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7">
         <v>15</v>
@@ -2307,7 +2360,7 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E9">
         <v>7.5</v>
@@ -2328,7 +2381,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11">
         <v>15</v>
@@ -2349,7 +2402,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E13">
         <v>25</v>
@@ -2359,7 +2412,7 @@
         <v>25000</v>
       </c>
       <c r="G13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -2374,12 +2427,12 @@
         <v>105000</v>
       </c>
       <c r="G14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E15">
         <v>16</v>
@@ -2389,49 +2442,49 @@
         <v>16000</v>
       </c>
       <c r="G15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -2439,26 +2492,26 @@
         <v>57</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" t="s">
         <v>160</v>
-      </c>
-      <c r="C23" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
last set of revisions before committee
almost done, yippee
</commit_message>
<xml_diff>
--- a/Data/Other SSY studies.xlsx
+++ b/Data/Other SSY studies.xlsx
@@ -806,8 +806,8 @@
       <xdr:rowOff>143289</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>437138</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2474659</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>114208</xdr:rowOff>
     </xdr:to>
@@ -845,7 +845,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>227968</xdr:colOff>
+      <xdr:colOff>227969</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
@@ -1219,16 +1219,16 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
@@ -1641,6 +1641,10 @@
       <c r="D23" s="4">
         <v>76000</v>
       </c>
+      <c r="F23">
+        <f>80000000/D23</f>
+        <v>1052.6315789473683</v>
+      </c>
       <c r="G23" t="s">
         <v>87</v>
       </c>
@@ -1660,6 +1664,10 @@
       </c>
       <c r="D24" s="4">
         <v>35000</v>
+      </c>
+      <c r="F24">
+        <f>105000000/D24</f>
+        <v>3000</v>
       </c>
       <c r="G24" t="s">
         <v>88</v>
@@ -1839,13 +1847,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="38.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
@@ -2125,8 +2133,8 @@
         <v>9.0000000000000007E-7</v>
       </c>
       <c r="H12" s="4">
-        <f>D12*(G12^E12)</f>
-        <v>515070.97357892909</v>
+        <f>D12*(F12^E12)</f>
+        <v>296.3924087604471</v>
       </c>
       <c r="I12">
         <v>1.78</v>
@@ -2160,8 +2168,8 @@
         <v>9.0000000000000007E-7</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" ref="H13:H16" si="4">D13*(G13^E13)</f>
-        <v>39261.040244045907</v>
+        <f t="shared" ref="H13:H16" si="4">D13*(F13^E13)</f>
+        <v>68.227868273665564</v>
       </c>
       <c r="I13">
         <v>1.78</v>
@@ -2196,7 +2204,7 @@
       </c>
       <c r="H14" s="4">
         <f t="shared" si="4"/>
-        <v>44276.997758483747</v>
+        <v>12.769625639933327</v>
       </c>
       <c r="I14" s="6">
         <v>1.78</v>
@@ -2231,7 +2239,7 @@
       </c>
       <c r="H15" s="4">
         <f t="shared" si="4"/>
-        <v>909.17510165613464</v>
+        <v>8.2917754758290574</v>
       </c>
       <c r="I15">
         <v>1.78</v>
@@ -2266,7 +2274,7 @@
       </c>
       <c r="H16" s="4">
         <f t="shared" si="4"/>
-        <v>80.932229138367319</v>
+        <v>5.1064784380006758</v>
       </c>
       <c r="I16">
         <v>1.78</v>

</xml_diff>